<commit_message>
partial update for the acceptance testing and customer order form
</commit_message>
<xml_diff>
--- a/documentation/buglist.xlsx
+++ b/documentation/buglist.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="153222"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\xampp-projects\OnlineOrdering\documentation\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\xampp_projects\OnlineOrdering\documentation\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -13,7 +13,8 @@
   </bookViews>
   <sheets>
     <sheet name="Bug" sheetId="1" r:id="rId1"/>
-    <sheet name="Versions" sheetId="2" r:id="rId2"/>
+    <sheet name="Enhancements" sheetId="3" r:id="rId2"/>
+    <sheet name="Versions" sheetId="2" r:id="rId3"/>
   </sheets>
   <calcPr calcId="152511"/>
   <extLst>
@@ -25,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12" uniqueCount="11">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="24" uniqueCount="19">
   <si>
     <t>Bug description</t>
   </si>
@@ -58,19 +59,49 @@
   </si>
   <si>
     <t>ie 11, edge only</t>
+  </si>
+  <si>
+    <t>I am entering an order and wanted to put in a percentage which was not a round number and the system auto rounded up on me. This will need to be changed as a lot of additives are not whole numbers. Can we change this please</t>
+  </si>
+  <si>
+    <t>All</t>
+  </si>
+  <si>
+    <t>Required Enhancement</t>
+  </si>
+  <si>
+    <t>Version</t>
+  </si>
+  <si>
+    <t>Standard Order Sheet Output</t>
+  </si>
+  <si>
+    <t>1.0.1</t>
+  </si>
+  <si>
+    <t>Modified View files accordingly</t>
+  </si>
+  <si>
+    <t xml:space="preserve">can't seem to get it to do the weighbridge ticket or print out or allow the despatching of the finished order. </t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <color rgb="FF000000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
     </font>
   </fonts>
   <fills count="2">
@@ -93,8 +124,14 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -375,22 +412,22 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:D2"/>
+  <dimension ref="A1:E4"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B2" sqref="B2"/>
+      <selection activeCell="A4" sqref="A4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="74.90625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="9.6328125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="18.453125" customWidth="1"/>
-    <col min="4" max="4" width="9.54296875" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="74.85546875" style="1" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="15" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="18.42578125" customWidth="1"/>
+    <col min="4" max="4" width="9.5703125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A1" t="s">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
       <c r="B1" t="s">
@@ -403,8 +440,8 @@
         <v>8</v>
       </c>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A2" t="s">
+    <row r="2" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+      <c r="A2" s="1" t="s">
         <v>2</v>
       </c>
       <c r="B2" t="s">
@@ -412,6 +449,69 @@
       </c>
       <c r="C2" t="s">
         <v>3</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" ht="45" x14ac:dyDescent="0.25">
+      <c r="A3" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="B3" t="s">
+        <v>12</v>
+      </c>
+      <c r="C3" t="s">
+        <v>3</v>
+      </c>
+      <c r="D3" t="s">
+        <v>16</v>
+      </c>
+      <c r="E3" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A4" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="B4" t="s">
+        <v>12</v>
+      </c>
+      <c r="C4" t="s">
+        <v>3</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:B2"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C2" sqref="C2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="31.85546875" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>13</v>
+      </c>
+      <c r="B1" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>15</v>
+      </c>
+      <c r="B2" t="s">
+        <v>16</v>
       </c>
     </row>
   </sheetData>
@@ -419,7 +519,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:C2"/>
   <sheetViews>
@@ -427,14 +527,14 @@
       <selection activeCell="C3" sqref="C3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="14.26953125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="39.54296875" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="72.54296875" customWidth="1"/>
+    <col min="1" max="1" width="14.28515625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="39.5703125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="72.5703125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>4</v>
       </c>
@@ -442,7 +542,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>3</v>
       </c>

</xml_diff>

<commit_message>
updated the action buttons
</commit_message>
<xml_diff>
--- a/documentation/buglist.xlsx
+++ b/documentation/buglist.xlsx
@@ -130,7 +130,7 @@
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment vertical="center"/>
+      <alignment vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -415,7 +415,7 @@
   <dimension ref="A1:E4"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A4" sqref="A4"/>
+      <selection activeCell="B4" sqref="B4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -468,7 +468,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="4" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:5" ht="31.5" x14ac:dyDescent="0.25">
       <c r="A4" s="2" t="s">
         <v>18</v>
       </c>

</xml_diff>

<commit_message>
Added Daily Sales Figures
</commit_message>
<xml_diff>
--- a/documentation/buglist.xlsx
+++ b/documentation/buglist.xlsx
@@ -5,15 +5,15 @@
   <workbookPr defaultThemeVersion="153222"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\xampp_projects\OnlineOrdering\documentation\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\xampp-projects\OnlineOrdering\documentation\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="21600" windowHeight="12210"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="21600" windowHeight="12210" activeTab="2"/>
   </bookViews>
   <sheets>
-    <sheet name="Bug" sheetId="1" r:id="rId1"/>
-    <sheet name="Enhancements" sheetId="3" r:id="rId2"/>
+    <sheet name="Bug List" sheetId="1" r:id="rId1"/>
+    <sheet name="Enhancements" sheetId="4" r:id="rId2"/>
     <sheet name="Versions" sheetId="2" r:id="rId3"/>
   </sheets>
   <calcPr calcId="152511"/>
@@ -26,14 +26,11 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="24" uniqueCount="19">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="37" uniqueCount="26">
   <si>
     <t>Bug description</t>
   </si>
   <si>
-    <t>Browser</t>
-  </si>
-  <si>
     <t>Cant add additional ingredients after the first. And the pjax reload not working correctly</t>
   </si>
   <si>
@@ -58,24 +55,9 @@
     <t>Version Found</t>
   </si>
   <si>
-    <t>ie 11, edge only</t>
-  </si>
-  <si>
     <t>I am entering an order and wanted to put in a percentage which was not a round number and the system auto rounded up on me. This will need to be changed as a lot of additives are not whole numbers. Can we change this please</t>
   </si>
   <si>
-    <t>All</t>
-  </si>
-  <si>
-    <t>Required Enhancement</t>
-  </si>
-  <si>
-    <t>Version</t>
-  </si>
-  <si>
-    <t>Standard Order Sheet Output</t>
-  </si>
-  <si>
     <t>1.0.1</t>
   </si>
   <si>
@@ -83,6 +65,45 @@
   </si>
   <si>
     <t xml:space="preserve">can't seem to get it to do the weighbridge ticket or print out or allow the despatching of the finished order. </t>
+  </si>
+  <si>
+    <t>Set the delivery details page to read only when completed</t>
+  </si>
+  <si>
+    <t>uncomplete a delivery needs to roll back to the last delivery details</t>
+  </si>
+  <si>
+    <t>Add Anticpated Sales in Dashboard and menu item</t>
+  </si>
+  <si>
+    <t>Order State Widget</t>
+  </si>
+  <si>
+    <t>1.0.2</t>
+  </si>
+  <si>
+    <t>Add Daily Sales Figures (Client,Ordered,Dispatched,returned,difference)</t>
+  </si>
+  <si>
+    <t>Details</t>
+  </si>
+  <si>
+    <t>Requested</t>
+  </si>
+  <si>
+    <t>Added in Version</t>
+  </si>
+  <si>
+    <t>f36ffae9f7b9fe5ba2b4286e5bb90c03bd9fd721</t>
+  </si>
+  <si>
+    <t>Finalised version before user testing</t>
+  </si>
+  <si>
+    <t>1.0.3</t>
+  </si>
+  <si>
+    <t>Added Daily Sales figures screen</t>
   </si>
 </sst>
 </file>
@@ -124,7 +145,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -132,6 +153,7 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -412,71 +434,94 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E4"/>
+  <dimension ref="A1:D7"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B4" sqref="B4"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D7" sqref="D7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="74.85546875" style="1" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="15" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="18.42578125" customWidth="1"/>
-    <col min="4" max="4" width="9.5703125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="18.42578125" customWidth="1"/>
+    <col min="3" max="3" width="13.28515625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
       <c r="B1" t="s">
+        <v>8</v>
+      </c>
+      <c r="C1" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" ht="30" x14ac:dyDescent="0.25">
+      <c r="A2" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="C1" t="s">
+      <c r="B2" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" ht="45" x14ac:dyDescent="0.25">
+      <c r="A3" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="D1" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="2" spans="1:5" ht="30" x14ac:dyDescent="0.25">
-      <c r="A2" s="1" t="s">
+      <c r="B3" t="s">
         <v>2</v>
       </c>
-      <c r="B2" t="s">
+      <c r="C3" t="s">
         <v>10</v>
       </c>
-      <c r="C2" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="3" spans="1:5" ht="45" x14ac:dyDescent="0.25">
-      <c r="A3" s="1" t="s">
+      <c r="D3" t="s">
         <v>11</v>
       </c>
-      <c r="B3" t="s">
+    </row>
+    <row r="4" spans="1:4" ht="31.5" x14ac:dyDescent="0.25">
+      <c r="A4" s="2" t="s">
         <v>12</v>
       </c>
-      <c r="C3" t="s">
-        <v>3</v>
-      </c>
-      <c r="D3" t="s">
-        <v>16</v>
-      </c>
-      <c r="E3" t="s">
+      <c r="B4" t="s">
+        <v>2</v>
+      </c>
+      <c r="C4" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A5" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="B5" t="s">
+        <v>10</v>
+      </c>
+      <c r="C5" t="s">
         <v>17</v>
       </c>
     </row>
-    <row r="4" spans="1:5" ht="31.5" x14ac:dyDescent="0.25">
-      <c r="A4" s="2" t="s">
-        <v>18</v>
-      </c>
-      <c r="B4" t="s">
-        <v>12</v>
-      </c>
-      <c r="C4" t="s">
-        <v>3</v>
+    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A6" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="B6" t="s">
+        <v>10</v>
+      </c>
+      <c r="C6" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A7" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="B7" t="s">
+        <v>10</v>
+      </c>
+      <c r="C7" t="s">
+        <v>17</v>
       </c>
     </row>
   </sheetData>
@@ -487,31 +532,44 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:B2"/>
+  <dimension ref="A1:C3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C2" sqref="C2"/>
+      <selection activeCell="C7" sqref="C7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="31.85546875" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="71.140625" customWidth="1"/>
+    <col min="2" max="2" width="9.7109375" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="16.42578125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>13</v>
+        <v>19</v>
       </c>
       <c r="B1" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A2" t="s">
-        <v>15</v>
-      </c>
-      <c r="B2" t="s">
+        <v>20</v>
+      </c>
+      <c r="C1" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A2" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="B2" s="3">
+        <v>42491</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A3" s="1" t="s">
         <v>16</v>
+      </c>
+      <c r="B3" s="3">
+        <v>42491</v>
       </c>
     </row>
   </sheetData>
@@ -521,36 +579,60 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:C2"/>
+  <dimension ref="A1:C5"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C3" sqref="C3"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B5" sqref="B5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="14.28515625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="39.5703125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="41.7109375" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="72.5703125" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
+        <v>3</v>
+      </c>
+      <c r="B1" t="s">
         <v>4</v>
-      </c>
-      <c r="B1" t="s">
-        <v>5</v>
       </c>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="B2" t="s">
+        <v>5</v>
+      </c>
+      <c r="C2" t="s">
         <v>6</v>
       </c>
-      <c r="C2" t="s">
-        <v>7</v>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>17</v>
+      </c>
+      <c r="B4" t="s">
+        <v>22</v>
+      </c>
+      <c r="C4" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>24</v>
+      </c>
+      <c r="C5" t="s">
+        <v>25</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Added the Order Status widget along the top of the display
Version 1.0.4 worked 4 hours
</commit_message>
<xml_diff>
--- a/documentation/buglist.xlsx
+++ b/documentation/buglist.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="21600" windowHeight="12210" activeTab="2"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="21600" windowHeight="12210"/>
   </bookViews>
   <sheets>
     <sheet name="Bug List" sheetId="1" r:id="rId1"/>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="37" uniqueCount="26">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="42" uniqueCount="29">
   <si>
     <t>Bug description</t>
   </si>
@@ -104,6 +104,15 @@
   </si>
   <si>
     <t>Added Daily Sales figures screen</t>
+  </si>
+  <si>
+    <t>6410c4d660bd46c7dd1254e7d8204dd9235d92ef</t>
+  </si>
+  <si>
+    <t>1.0.4</t>
+  </si>
+  <si>
+    <t>Added the order status widget along the top</t>
   </si>
 </sst>
 </file>
@@ -436,7 +445,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D7"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="D7" sqref="D7"/>
     </sheetView>
   </sheetViews>
@@ -535,7 +544,7 @@
   <dimension ref="A1:C3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C7" sqref="C7"/>
+      <selection activeCell="C3" sqref="C3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -563,6 +572,9 @@
       <c r="B2" s="3">
         <v>42491</v>
       </c>
+      <c r="C2" t="s">
+        <v>24</v>
+      </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
@@ -570,6 +582,9 @@
       </c>
       <c r="B3" s="3">
         <v>42491</v>
+      </c>
+      <c r="C3" t="s">
+        <v>27</v>
       </c>
     </row>
   </sheetData>
@@ -579,10 +594,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:C5"/>
+  <dimension ref="A1:C6"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B5" sqref="B5"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B6" sqref="B6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -631,8 +646,19 @@
       <c r="A5" t="s">
         <v>24</v>
       </c>
+      <c r="B5" t="s">
+        <v>26</v>
+      </c>
       <c r="C5" t="s">
         <v>25</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>27</v>
+      </c>
+      <c r="C6" t="s">
+        <v>28</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Updated the bug lists, and enhancements
2 Hours work
</commit_message>
<xml_diff>
--- a/documentation/buglist.xlsx
+++ b/documentation/buglist.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="153222"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\xampp-projects\OnlineOrdering\documentation\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\xampp_projects\OnlineOrdering\documentation\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="44" uniqueCount="31">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="50" uniqueCount="34">
   <si>
     <t>Bug description</t>
   </si>
@@ -119,6 +119,15 @@
   </si>
   <si>
     <t>Change the default fill method to select bins first</t>
+  </si>
+  <si>
+    <t>Add in the label printing to the delivery sheet</t>
+  </si>
+  <si>
+    <t>1.0.5</t>
+  </si>
+  <si>
+    <t>Bug fixes (See Bug List) and adding the labels</t>
   </si>
 </sst>
 </file>
@@ -452,7 +461,7 @@
   <dimension ref="A1:D7"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D7" sqref="D7"/>
+      <selection activeCell="A8" sqref="A8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -547,10 +556,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:C5"/>
+  <dimension ref="A1:C6"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A11" sqref="A11"/>
+      <selection activeCell="A6" sqref="A6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -600,6 +609,9 @@
       <c r="B4" s="3">
         <v>42499</v>
       </c>
+      <c r="C4" t="s">
+        <v>32</v>
+      </c>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
@@ -607,6 +619,20 @@
       </c>
       <c r="B5" s="3">
         <v>42499</v>
+      </c>
+      <c r="C5" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>31</v>
+      </c>
+      <c r="B6" s="3">
+        <v>42499</v>
+      </c>
+      <c r="C6" t="s">
+        <v>32</v>
       </c>
     </row>
   </sheetData>
@@ -616,10 +642,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:C6"/>
+  <dimension ref="A1:C7"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B6" sqref="B6"/>
+      <selection activeCell="C7" sqref="C7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -683,6 +709,14 @@
         <v>28</v>
       </c>
     </row>
+    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
+        <v>32</v>
+      </c>
+      <c r="C7" t="s">
+        <v>33</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
Updates using bug fixes
</commit_message>
<xml_diff>
--- a/documentation/buglist.xlsx
+++ b/documentation/buglist.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="21600" windowHeight="12210" activeTab="1"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="21600" windowHeight="12210"/>
   </bookViews>
   <sheets>
     <sheet name="Bug List" sheetId="1" r:id="rId1"/>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="50" uniqueCount="34">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="58" uniqueCount="39">
   <si>
     <t>Bug description</t>
   </si>
@@ -128,6 +128,21 @@
   </si>
   <si>
     <t>Bug fixes (See Bug List) and adding the labels</t>
+  </si>
+  <si>
+    <t>Add in the trailer name to the Paired with trailer screen not just the rego number</t>
+  </si>
+  <si>
+    <t>1.0.6</t>
+  </si>
+  <si>
+    <t>Display the Trailer pair and tdefault truck in the index page for trailers</t>
+  </si>
+  <si>
+    <t>Customer orer sheet displays XX in truck type</t>
+  </si>
+  <si>
+    <t>Customer order sheet to be emailed on submit</t>
   </si>
 </sst>
 </file>
@@ -458,10 +473,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:D7"/>
+  <dimension ref="A1:D11"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A8" sqref="A8"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B11" sqref="B11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -548,6 +563,38 @@
         <v>17</v>
       </c>
     </row>
+    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A8" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="B8" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A9" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="B9" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A10" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="B10" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A11" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="B11" t="s">
+        <v>35</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
@@ -558,7 +605,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:C6"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="A6" sqref="A6"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
started update to the delivery allocation screen
</commit_message>
<xml_diff>
--- a/documentation/buglist.xlsx
+++ b/documentation/buglist.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="21600" windowHeight="12210" activeTab="2"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="21600" windowHeight="12210"/>
   </bookViews>
   <sheets>
     <sheet name="Bug List" sheetId="1" r:id="rId1"/>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="67" uniqueCount="41">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="77" uniqueCount="46">
   <si>
     <t>Bug description</t>
   </si>
@@ -149,6 +149,21 @@
   </si>
   <si>
     <t>Added email Queues and minor bug fixes</t>
+  </si>
+  <si>
+    <t>Dummy account appears in the order status widget when creating a new order</t>
+  </si>
+  <si>
+    <t>when customer is on hold, prevent orders being created</t>
+  </si>
+  <si>
+    <t>remove the bin description from the loader sheet</t>
+  </si>
+  <si>
+    <t>create a separate sheet for additivies</t>
+  </si>
+  <si>
+    <t>change the deliery page to selec the truck first</t>
   </si>
 </sst>
 </file>
@@ -479,10 +494,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:D12"/>
+  <dimension ref="A1:D17"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C9" sqref="C9:C12"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C17" sqref="C17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -621,6 +636,46 @@
         <v>32</v>
       </c>
       <c r="C12" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="13" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A13" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="B13" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="14" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A14" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="B14" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="15" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A15" s="1" t="s">
+        <v>43</v>
+      </c>
+      <c r="B15" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="16" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A16" s="1" t="s">
+        <v>44</v>
+      </c>
+      <c r="B16" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="17" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A17" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="B17" t="s">
         <v>35</v>
       </c>
     </row>
@@ -720,7 +775,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:C8"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="C8" sqref="C8"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
Update 1.0.7 See log file for details
3 Hours Work
</commit_message>
<xml_diff>
--- a/documentation/buglist.xlsx
+++ b/documentation/buglist.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="153222"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\xampp_projects\OnlineOrdering\documentation\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\xampp-projects\OnlineOrdering\documentation\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="82" uniqueCount="48">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="85" uniqueCount="48">
   <si>
     <t>Bug description</t>
   </si>
@@ -503,7 +503,7 @@
   <dimension ref="A1:D18"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B18" sqref="B18"/>
+      <selection activeCell="D18" sqref="D18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -663,6 +663,9 @@
       <c r="B14" t="s">
         <v>35</v>
       </c>
+      <c r="C14" t="s">
+        <v>46</v>
+      </c>
     </row>
     <row r="15" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A15" s="1" t="s">
@@ -671,6 +674,9 @@
       <c r="B15" t="s">
         <v>35</v>
       </c>
+      <c r="C15" t="s">
+        <v>46</v>
+      </c>
     </row>
     <row r="16" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A16" s="1" t="s">
@@ -700,6 +706,9 @@
       </c>
       <c r="B18" t="s">
         <v>35</v>
+      </c>
+      <c r="C18" t="s">
+        <v>46</v>
       </c>
     </row>
   </sheetData>

</xml_diff>